<commit_message>
HomeMove submit button added
</commit_message>
<xml_diff>
--- a/Selenium-Scripts/src/appConfigFileHomeMove.xlsx
+++ b/Selenium-Scripts/src/appConfigFileHomeMove.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="HomePage" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="79">
   <si>
     <t>Key</t>
   </si>
@@ -258,6 +258,12 @@
   </si>
   <si>
     <t>//android.widget.TextView[@text='Home move']</t>
+  </si>
+  <si>
+    <t>//android.widget.Button[@resource-id='com.Etisalat.ETIDA:id/btn_submit_request']</t>
+  </si>
+  <si>
+    <t>submitButton</t>
   </si>
 </sst>
 </file>
@@ -670,7 +676,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
@@ -1011,10 +1017,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1109,6 +1115,14 @@
       </c>
       <c r="B11" t="s">
         <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>78</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>